<commit_message>
simple dashboard deployed with improved features in excel
</commit_message>
<xml_diff>
--- a/attendance_backup.xlsx
+++ b/attendance_backup.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Face Recognition Attendance" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,17 +27,36 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="008DB4E2"/>
+        <bgColor rgb="008DB4E2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,20 +64,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,166 +441,394 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>DATE</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>hameed</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>linguuu</t>
-        </is>
-      </c>
+          <t>HAMEED</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>naveed</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>rizwana</t>
-        </is>
-      </c>
+          <t>LINGUUU</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>sajjad</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>sammm</t>
-        </is>
-      </c>
+          <t>NAVEED</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n"/>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>vikinesh</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>yaseen</t>
-        </is>
-      </c>
+          <t>RIZWANA</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SAJJAD</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>SAMMM</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>VIKINESH</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>YASEEN</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-08-30</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>10:30:15</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>09:15:30</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>09:20:45</t>
+      <c r="A2" s="2" t="n"/>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>First Arrival</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Latest Visit</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>First Arrival</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Latest Visit</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>First Arrival</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>Latest Visit</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>First Arrival</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>Latest Visit</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>First Arrival</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>Latest Visit</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>First Arrival</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>Latest Visit</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>First Arrival</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>Latest Visit</t>
+        </is>
+      </c>
+      <c r="P2" s="2" t="inlineStr">
+        <is>
+          <t>First Arrival</t>
+        </is>
+      </c>
+      <c r="Q2" s="2" t="inlineStr">
+        <is>
+          <t>Latest Visit</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-08-31</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>09:10:30</t>
-        </is>
-      </c>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>19:37:51</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>11:15:45</t>
-        </is>
-      </c>
+          <t>10:30:15</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>10:30:15</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>09:15:30</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>09:15:30</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>09:20:45</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>09:20:45</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>09:10:30</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>11:35:32</t>
+          <t>09:10:30</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>11:36:21</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>11:36:21</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>19:37:51</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>19:37:51</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>11:15:45</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>11:15:45</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-09-20</t>
+          <t>2025-09-01</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>11:35:32</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>01:23:03</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>01:23:05</t>
-        </is>
-      </c>
+          <t>11:35:32</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>11:36:21</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>11:36:21</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>11:36:21</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>11:36:21</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>01:23:03</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>01:23:03</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>01:23:05</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>01:23:05</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-09-21</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>14:55:16</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>20:25:28</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>